<commit_message>
Created a product feature list (documentation folder) Enabled logging via email when a user tries to login
</commit_message>
<xml_diff>
--- a/Documentation/Product features.xlsx
+++ b/Documentation/Product features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>internationalization</t>
+  </si>
+  <si>
+    <t>log attempts in database and send via email when an error (or above) happens</t>
+  </si>
+  <si>
+    <t>be able to create, delete and edit other users. The simple users will only be able to edit their data (except from their category)</t>
   </si>
 </sst>
 </file>
@@ -479,7 +485,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +495,7 @@
     <col min="3" max="3" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="15" style="3" customWidth="1"/>
     <col min="8" max="8" width="14" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -537,7 +543,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>12</v>
@@ -634,9 +640,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -743,7 +758,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Class refactoring. Created the table for log records
</commit_message>
<xml_diff>
--- a/Documentation/Product features.xlsx
+++ b/Documentation/Product features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>be able to create, delete and edit other users. The simple users will only be able to edit their data (except from their category)</t>
+  </si>
+  <si>
+    <t>to properly insert the organizational chart in the database</t>
   </si>
 </sst>
 </file>
@@ -485,7 +488,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -626,7 +629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -654,9 +657,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Minor changes to the documentation
</commit_message>
<xml_diff>
--- a/Documentation/Product features.xlsx
+++ b/Documentation/Product features.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -82,9 +82,6 @@
     <t>As a/an</t>
   </si>
   <si>
-    <t>log attempts in database and send via email</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -100,12 +97,6 @@
     <t>Non functional</t>
   </si>
   <si>
-    <t>add slashes to URL's</t>
-  </si>
-  <si>
-    <t>the user can navigate more easily</t>
-  </si>
-  <si>
     <t>redesign code using the MVC pattern</t>
   </si>
   <si>
@@ -131,6 +122,9 @@
   </si>
   <si>
     <t>to properly insert the organizational chart in the database</t>
+  </si>
+  <si>
+    <t>code was restructured (MVT pattern)</t>
   </si>
 </sst>
 </file>
@@ -188,8 +182,36 @@
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -485,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,13 +568,13 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -563,16 +585,16 @@
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>11</v>
@@ -581,32 +603,35 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>27</v>
+      <c r="F4" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>15</v>
@@ -614,10 +639,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>29</v>
@@ -625,123 +650,106 @@
       <c r="F6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
         <v>24</v>
       </c>
     </row>
@@ -761,10 +769,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,64 +814,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>